<commit_message>
ui fixes and category addition
</commit_message>
<xml_diff>
--- a/public/sample.xlsx
+++ b/public/sample.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B47948E-AD8F-4724-A71F-EFC4E782EDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CF2B3A-5925-4C41-9E11-2C229F65EE9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4830" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-4830" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APR-25" sheetId="1" r:id="rId1"/>
@@ -2452,7 +2452,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="72">
   <si>
     <t>Date</t>
   </si>
@@ -2666,6 +2666,9 @@
   <si>
     <t>Punching Rejection %</t>
   </si>
+  <si>
+    <t>Solar Generation (NEW) 214(menus)</t>
+  </si>
 </sst>
 </file>
 
@@ -2814,7 +2817,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2854,6 +2857,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2918,7 +2933,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3132,49 +3147,31 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3462,9 +3459,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL107"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A42" sqref="A42"/>
+      <selection pane="topRight" activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4822,7 +4819,7 @@
       <c r="AJ16" s="22"/>
     </row>
     <row r="17" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="77" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="8">
@@ -5871,7 +5868,7 @@
       <c r="AJ27" s="22"/>
     </row>
     <row r="28" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="77" t="s">
         <v>23</v>
       </c>
       <c r="B28" s="27">
@@ -5998,7 +5995,7 @@
       <c r="AJ28" s="22"/>
     </row>
     <row r="29" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
+      <c r="A29" s="78"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -7118,7 +7115,7 @@
       <c r="AI42" s="16"/>
     </row>
     <row r="43" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="7"/>
+      <c r="A43" s="78"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
@@ -7673,7 +7670,7 @@
       <c r="AI48" s="9"/>
     </row>
     <row r="49" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="7"/>
+      <c r="A49" s="78"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
@@ -7860,7 +7857,7 @@
       <c r="AI53" s="9"/>
     </row>
     <row r="54" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A54" s="17"/>
+      <c r="A54" s="84"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
@@ -8126,7 +8123,7 @@
       <c r="AI57" s="9"/>
     </row>
     <row r="58" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A58" s="65" t="s">
+      <c r="A58" s="79" t="s">
         <v>45</v>
       </c>
       <c r="B58" s="8">
@@ -8223,7 +8220,7 @@
       <c r="AI58" s="9"/>
     </row>
     <row r="59" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A59" s="35" t="s">
+      <c r="A59" s="79" t="s">
         <v>46</v>
       </c>
       <c r="B59" s="8">
@@ -8320,7 +8317,7 @@
       <c r="AI59" s="9"/>
     </row>
     <row r="60" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A60" s="66" t="s">
+      <c r="A60" s="79" t="s">
         <v>47</v>
       </c>
       <c r="B60" s="8">
@@ -8417,7 +8414,7 @@
       <c r="AI60" s="9"/>
     </row>
     <row r="61" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="80" t="s">
         <v>48</v>
       </c>
       <c r="B61" s="36">
@@ -8546,7 +8543,7 @@
       <c r="AI61" s="69"/>
     </row>
     <row r="62" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="7"/>
+      <c r="A62" s="78"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
@@ -8678,7 +8675,7 @@
       <c r="AI63" s="9"/>
     </row>
     <row r="64" spans="1:35" ht="18" x14ac:dyDescent="0.3">
-      <c r="A64" s="33" t="s">
+      <c r="A64" s="81" t="s">
         <v>50</v>
       </c>
       <c r="B64" s="8">
@@ -8775,7 +8772,7 @@
       <c r="AI64" s="9"/>
     </row>
     <row r="65" spans="1:35" ht="18" x14ac:dyDescent="0.3">
-      <c r="A65" s="64" t="s">
+      <c r="A65" s="82" t="s">
         <v>51</v>
       </c>
       <c r="B65" s="8">
@@ -8872,7 +8869,7 @@
       <c r="AI65" s="9"/>
     </row>
     <row r="66" spans="1:35" ht="18" x14ac:dyDescent="0.3">
-      <c r="A66" s="64" t="s">
+      <c r="A66" s="82" t="s">
         <v>69</v>
       </c>
       <c r="B66" s="15">
@@ -9000,7 +8997,7 @@
       <c r="AI66" s="16"/>
     </row>
     <row r="67" spans="1:35" ht="18" x14ac:dyDescent="0.3">
-      <c r="A67" s="34"/>
+      <c r="A67" s="83"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
@@ -9132,7 +9129,7 @@
       <c r="AI68" s="9"/>
     </row>
     <row r="69" spans="1:35" ht="18" x14ac:dyDescent="0.3">
-      <c r="A69" s="34"/>
+      <c r="A69" s="83"/>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
@@ -9402,7 +9399,7 @@
       <c r="AI72" s="40"/>
     </row>
     <row r="73" spans="1:35" ht="18" x14ac:dyDescent="0.3">
-      <c r="A73" s="34"/>
+      <c r="A73" s="83"/>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
@@ -9437,8 +9434,8 @@
       <c r="AI73" s="9"/>
     </row>
     <row r="74" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="10" t="s">
-        <v>56</v>
+      <c r="A74" s="80" t="s">
+        <v>71</v>
       </c>
       <c r="B74" s="8">
         <v>0</v>
@@ -9534,7 +9531,7 @@
       <c r="AI74" s="9"/>
     </row>
     <row r="75" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="10" t="s">
+      <c r="A75" s="80" t="s">
         <v>57</v>
       </c>
       <c r="B75" s="8">
@@ -9631,7 +9628,7 @@
       <c r="AI75" s="9"/>
     </row>
     <row r="76" spans="1:35" ht="18" x14ac:dyDescent="0.3">
-      <c r="A76" s="33" t="s">
+      <c r="A76" s="81" t="s">
         <v>58</v>
       </c>
       <c r="B76" s="8">
@@ -9728,7 +9725,7 @@
       <c r="AI76" s="9"/>
     </row>
     <row r="77" spans="1:35" ht="18" x14ac:dyDescent="0.3">
-      <c r="A77" s="33" t="s">
+      <c r="A77" s="81" t="s">
         <v>59</v>
       </c>
       <c r="B77" s="8">
@@ -9825,7 +9822,7 @@
       <c r="AI77" s="9"/>
     </row>
     <row r="78" spans="1:35" ht="18" x14ac:dyDescent="0.3">
-      <c r="A78" s="33" t="s">
+      <c r="A78" s="81" t="s">
         <v>68</v>
       </c>
       <c r="B78" s="8">
@@ -9922,7 +9919,7 @@
       <c r="AI78" s="9"/>
     </row>
     <row r="79" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A79" s="41"/>
+      <c r="A79" s="85"/>
     </row>
     <row r="80" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A80" s="41"/>
@@ -9965,7 +9962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AL107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="D45" sqref="D45"/>
     </sheetView>
@@ -17402,9 +17399,8 @@
       </c>
       <c r="AF1" s="59"/>
       <c r="AG1" s="59"/>
-      <c r="AH1" s="89"/>
-      <c r="AI1" s="92"/>
-      <c r="AJ1" s="93"/>
+      <c r="AH1" s="59"/>
+      <c r="AI1" s="68"/>
       <c r="AK1" s="9"/>
     </row>
     <row r="2" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
@@ -17441,9 +17437,7 @@
       <c r="AE2" s="49"/>
       <c r="AF2" s="9"/>
       <c r="AG2" s="9"/>
-      <c r="AH2" s="77"/>
-      <c r="AI2" s="93"/>
-      <c r="AJ2" s="93"/>
+      <c r="AH2" s="9"/>
     </row>
     <row r="3" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="73" t="s">
@@ -17539,9 +17533,7 @@
       <c r="AE3" s="49"/>
       <c r="AF3" s="9"/>
       <c r="AG3" s="9"/>
-      <c r="AH3" s="77"/>
-      <c r="AI3" s="78"/>
-      <c r="AJ3" s="78"/>
+      <c r="AH3" s="9"/>
     </row>
     <row r="4" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="23" t="s">
@@ -17595,9 +17587,7 @@
       <c r="AE4" s="49"/>
       <c r="AF4" s="9"/>
       <c r="AG4" s="9"/>
-      <c r="AH4" s="77"/>
-      <c r="AI4" s="78"/>
-      <c r="AJ4" s="78"/>
+      <c r="AH4" s="9"/>
     </row>
     <row r="5" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
@@ -17651,9 +17641,7 @@
       <c r="AE5" s="49"/>
       <c r="AF5" s="9"/>
       <c r="AG5" s="9"/>
-      <c r="AH5" s="77"/>
-      <c r="AI5" s="78"/>
-      <c r="AJ5" s="78"/>
+      <c r="AH5" s="9"/>
     </row>
     <row r="6" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
@@ -17749,9 +17737,7 @@
       <c r="AE6" s="49"/>
       <c r="AF6" s="9"/>
       <c r="AG6" s="9"/>
-      <c r="AH6" s="77"/>
-      <c r="AI6" s="78"/>
-      <c r="AJ6" s="78"/>
+      <c r="AH6" s="9"/>
     </row>
     <row r="7" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
@@ -17847,9 +17833,8 @@
       <c r="AE7" s="49"/>
       <c r="AF7" s="9"/>
       <c r="AG7" s="9"/>
-      <c r="AH7" s="77"/>
-      <c r="AI7" s="79"/>
-      <c r="AJ7" s="78"/>
+      <c r="AH7" s="9"/>
+      <c r="AI7" s="47"/>
     </row>
     <row r="8" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
@@ -17943,9 +17928,7 @@
       <c r="AE8" s="49"/>
       <c r="AF8" s="9"/>
       <c r="AG8" s="9"/>
-      <c r="AH8" s="77"/>
-      <c r="AI8" s="78"/>
-      <c r="AJ8" s="78"/>
+      <c r="AH8" s="9"/>
     </row>
     <row r="9" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
@@ -18066,9 +18049,7 @@
       <c r="AE9" s="50"/>
       <c r="AF9" s="12"/>
       <c r="AG9" s="12"/>
-      <c r="AH9" s="80"/>
-      <c r="AI9" s="78"/>
-      <c r="AJ9" s="78"/>
+      <c r="AH9" s="12"/>
     </row>
     <row r="10" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
@@ -18162,9 +18143,7 @@
       <c r="AE10" s="49"/>
       <c r="AF10" s="9"/>
       <c r="AG10" s="9"/>
-      <c r="AH10" s="77"/>
-      <c r="AI10" s="78"/>
-      <c r="AJ10" s="78"/>
+      <c r="AH10" s="9"/>
     </row>
     <row r="11" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
@@ -18285,9 +18264,7 @@
       <c r="AE11" s="51"/>
       <c r="AF11" s="16"/>
       <c r="AG11" s="16"/>
-      <c r="AH11" s="81"/>
-      <c r="AI11" s="78"/>
-      <c r="AJ11" s="78"/>
+      <c r="AH11" s="16"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12" s="63" t="s">
@@ -18381,9 +18358,8 @@
       <c r="AE12" s="52"/>
       <c r="AF12" s="60"/>
       <c r="AG12" s="60"/>
-      <c r="AH12" s="90"/>
-      <c r="AI12" s="91"/>
-      <c r="AJ12" s="78"/>
+      <c r="AH12" s="60"/>
+      <c r="AI12" s="21"/>
       <c r="AK12" s="21"/>
     </row>
     <row r="13" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
@@ -18480,9 +18456,8 @@
       <c r="AE13" s="49"/>
       <c r="AF13" s="9"/>
       <c r="AG13" s="9"/>
-      <c r="AH13" s="77"/>
-      <c r="AI13" s="82"/>
-      <c r="AJ13" s="78"/>
+      <c r="AH13" s="9"/>
+      <c r="AI13" s="22"/>
     </row>
     <row r="14" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="23" t="s">
@@ -18578,9 +18553,8 @@
       <c r="AE14" s="49"/>
       <c r="AF14" s="9"/>
       <c r="AG14" s="9"/>
-      <c r="AH14" s="77"/>
-      <c r="AI14" s="82"/>
-      <c r="AJ14" s="78"/>
+      <c r="AH14" s="9"/>
+      <c r="AI14" s="22"/>
     </row>
     <row r="15" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
@@ -18676,9 +18650,8 @@
       <c r="AE15" s="49"/>
       <c r="AF15" s="9"/>
       <c r="AG15" s="9"/>
-      <c r="AH15" s="77"/>
-      <c r="AI15" s="82"/>
-      <c r="AJ15" s="78"/>
+      <c r="AH15" s="9"/>
+      <c r="AI15" s="22"/>
     </row>
     <row r="16" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
@@ -18714,11 +18687,10 @@
       <c r="AE16" s="49"/>
       <c r="AF16" s="9"/>
       <c r="AG16" s="9"/>
-      <c r="AH16" s="77"/>
-      <c r="AI16" s="82"/>
-      <c r="AJ16" s="78"/>
-    </row>
-    <row r="17" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH16" s="9"/>
+      <c r="AI16" s="22"/>
+    </row>
+    <row r="17" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="23" t="s">
         <v>13</v>
       </c>
@@ -18812,11 +18784,10 @@
       <c r="AE17" s="49"/>
       <c r="AF17" s="9"/>
       <c r="AG17" s="9"/>
-      <c r="AH17" s="77"/>
-      <c r="AI17" s="82"/>
-      <c r="AJ17" s="78"/>
-    </row>
-    <row r="18" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH17" s="9"/>
+      <c r="AI17" s="22"/>
+    </row>
+    <row r="18" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="s">
         <v>14</v>
       </c>
@@ -18910,11 +18881,10 @@
       <c r="AE18" s="49"/>
       <c r="AF18" s="9"/>
       <c r="AG18" s="9"/>
-      <c r="AH18" s="77"/>
-      <c r="AI18" s="82"/>
-      <c r="AJ18" s="78"/>
-    </row>
-    <row r="19" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH18" s="9"/>
+      <c r="AI18" s="22"/>
+    </row>
+    <row r="19" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="23" t="s">
         <v>15</v>
       </c>
@@ -19008,11 +18978,10 @@
       <c r="AE19" s="49"/>
       <c r="AF19" s="9"/>
       <c r="AG19" s="9"/>
-      <c r="AH19" s="77"/>
-      <c r="AI19" s="82"/>
-      <c r="AJ19" s="78"/>
-    </row>
-    <row r="20" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH19" s="9"/>
+      <c r="AI19" s="22"/>
+    </row>
+    <row r="20" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="23" t="s">
         <v>16</v>
       </c>
@@ -19106,11 +19075,10 @@
       <c r="AE20" s="49"/>
       <c r="AF20" s="9"/>
       <c r="AG20" s="9"/>
-      <c r="AH20" s="77"/>
-      <c r="AI20" s="82"/>
-      <c r="AJ20" s="78"/>
-    </row>
-    <row r="21" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH20" s="9"/>
+      <c r="AI20" s="22"/>
+    </row>
+    <row r="21" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="23" t="s">
         <v>17</v>
       </c>
@@ -19204,11 +19172,10 @@
       <c r="AE21" s="49"/>
       <c r="AF21" s="9"/>
       <c r="AG21" s="9"/>
-      <c r="AH21" s="77"/>
-      <c r="AI21" s="82"/>
-      <c r="AJ21" s="78"/>
-    </row>
-    <row r="22" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH21" s="9"/>
+      <c r="AI21" s="22"/>
+    </row>
+    <row r="22" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="23" t="s">
         <v>18</v>
       </c>
@@ -19302,11 +19269,10 @@
       <c r="AE22" s="49"/>
       <c r="AF22" s="9"/>
       <c r="AG22" s="9"/>
-      <c r="AH22" s="77"/>
-      <c r="AI22" s="82"/>
-      <c r="AJ22" s="78"/>
-    </row>
-    <row r="23" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH22" s="9"/>
+      <c r="AI22" s="22"/>
+    </row>
+    <row r="23" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -19340,11 +19306,10 @@
       <c r="AE23" s="49"/>
       <c r="AF23" s="9"/>
       <c r="AG23" s="9"/>
-      <c r="AH23" s="77"/>
-      <c r="AI23" s="82"/>
-      <c r="AJ23" s="78"/>
-    </row>
-    <row r="24" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH23" s="9"/>
+      <c r="AI23" s="22"/>
+    </row>
+    <row r="24" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="23" t="s">
         <v>19</v>
       </c>
@@ -19438,11 +19403,10 @@
       <c r="AE24" s="49"/>
       <c r="AF24" s="9"/>
       <c r="AG24" s="9"/>
-      <c r="AH24" s="77"/>
-      <c r="AI24" s="82"/>
-      <c r="AJ24" s="78"/>
-    </row>
-    <row r="25" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH24" s="9"/>
+      <c r="AI24" s="22"/>
+    </row>
+    <row r="25" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="73" t="s">
         <v>20</v>
       </c>
@@ -19536,11 +19500,10 @@
       <c r="AE25" s="49"/>
       <c r="AF25" s="9"/>
       <c r="AG25" s="9"/>
-      <c r="AH25" s="77"/>
-      <c r="AI25" s="82"/>
-      <c r="AJ25" s="78"/>
-    </row>
-    <row r="26" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH25" s="9"/>
+      <c r="AI25" s="22"/>
+    </row>
+    <row r="26" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="73" t="s">
         <v>21</v>
       </c>
@@ -19661,11 +19624,10 @@
       <c r="AE26" s="53"/>
       <c r="AF26" s="61"/>
       <c r="AG26" s="61"/>
-      <c r="AH26" s="83"/>
-      <c r="AI26" s="82"/>
-      <c r="AJ26" s="78"/>
-    </row>
-    <row r="27" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH26" s="26"/>
+      <c r="AI26" s="22"/>
+    </row>
+    <row r="27" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="73" t="s">
         <v>22</v>
       </c>
@@ -19759,11 +19721,10 @@
       <c r="AE27" s="54"/>
       <c r="AF27" s="26"/>
       <c r="AG27" s="26"/>
-      <c r="AH27" s="83"/>
-      <c r="AI27" s="82"/>
-      <c r="AJ27" s="78"/>
-    </row>
-    <row r="28" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AH27" s="26"/>
+      <c r="AI27" s="22"/>
+    </row>
+    <row r="28" spans="1:35" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="23" t="s">
         <v>23</v>
       </c>
@@ -19881,11 +19842,10 @@
       <c r="AE28" s="55"/>
       <c r="AF28" s="28"/>
       <c r="AG28" s="28"/>
-      <c r="AH28" s="84"/>
-      <c r="AI28" s="82"/>
-      <c r="AJ28" s="78"/>
-    </row>
-    <row r="29" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH28" s="28"/>
+      <c r="AI28" s="22"/>
+    </row>
+    <row r="29" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -19919,11 +19879,10 @@
       <c r="AE29" s="49"/>
       <c r="AF29" s="9"/>
       <c r="AG29" s="9"/>
-      <c r="AH29" s="77"/>
-      <c r="AI29" s="82"/>
-      <c r="AJ29" s="78"/>
-    </row>
-    <row r="30" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH29" s="9"/>
+      <c r="AI29" s="22"/>
+    </row>
+    <row r="30" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="73" t="s">
         <v>24</v>
       </c>
@@ -20017,11 +19976,10 @@
       <c r="AE30" s="49"/>
       <c r="AF30" s="9"/>
       <c r="AG30" s="9"/>
-      <c r="AH30" s="77"/>
-      <c r="AI30" s="82"/>
-      <c r="AJ30" s="78"/>
-    </row>
-    <row r="31" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH30" s="9"/>
+      <c r="AI30" s="22"/>
+    </row>
+    <row r="31" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="73" t="s">
         <v>25</v>
       </c>
@@ -20139,11 +20097,10 @@
       <c r="AE31" s="51"/>
       <c r="AF31" s="16"/>
       <c r="AG31" s="16"/>
-      <c r="AH31" s="81"/>
-      <c r="AI31" s="82"/>
-      <c r="AJ31" s="78"/>
-    </row>
-    <row r="32" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH31" s="16"/>
+      <c r="AI31" s="22"/>
+    </row>
+    <row r="32" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -20177,9 +20134,8 @@
       <c r="AE32" s="49"/>
       <c r="AF32" s="9"/>
       <c r="AG32" s="9"/>
-      <c r="AH32" s="77"/>
-      <c r="AI32" s="82"/>
-      <c r="AJ32" s="78"/>
+      <c r="AH32" s="9"/>
+      <c r="AI32" s="22"/>
     </row>
     <row r="33" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
@@ -20267,9 +20223,8 @@
       <c r="AE33" s="49"/>
       <c r="AF33" s="9"/>
       <c r="AG33" s="9"/>
-      <c r="AH33" s="77"/>
-      <c r="AI33" s="82"/>
-      <c r="AJ33" s="78"/>
+      <c r="AH33" s="9"/>
+      <c r="AI33" s="22"/>
     </row>
     <row r="34" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
@@ -20357,9 +20312,8 @@
       <c r="AE34" s="49"/>
       <c r="AF34" s="9"/>
       <c r="AG34" s="9"/>
-      <c r="AH34" s="77"/>
-      <c r="AI34" s="82"/>
-      <c r="AJ34" s="78"/>
+      <c r="AH34" s="9"/>
+      <c r="AI34" s="22"/>
     </row>
     <row r="35" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
@@ -20397,9 +20351,7 @@
       <c r="AE35" s="49"/>
       <c r="AF35" s="9"/>
       <c r="AG35" s="9"/>
-      <c r="AH35" s="77"/>
-      <c r="AI35" s="78"/>
-      <c r="AJ35" s="78"/>
+      <c r="AH35" s="9"/>
     </row>
     <row r="36" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
@@ -20435,9 +20387,8 @@
       <c r="AE36" s="49"/>
       <c r="AF36" s="9"/>
       <c r="AG36" s="9"/>
-      <c r="AH36" s="77"/>
-      <c r="AI36" s="82"/>
-      <c r="AJ36" s="78"/>
+      <c r="AH36" s="9"/>
+      <c r="AI36" s="22"/>
     </row>
     <row r="37" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="23" t="s">
@@ -20533,9 +20484,7 @@
       <c r="AE37" s="49"/>
       <c r="AF37" s="9"/>
       <c r="AG37" s="9"/>
-      <c r="AH37" s="77"/>
-      <c r="AI37" s="78"/>
-      <c r="AJ37" s="78"/>
+      <c r="AH37" s="9"/>
     </row>
     <row r="38" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
@@ -20571,9 +20520,8 @@
       <c r="AE38" s="49"/>
       <c r="AF38" s="9"/>
       <c r="AG38" s="9"/>
-      <c r="AH38" s="77"/>
-      <c r="AI38" s="82"/>
-      <c r="AJ38" s="78"/>
+      <c r="AH38" s="9"/>
+      <c r="AI38" s="22"/>
     </row>
     <row r="39" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="74" t="s">
@@ -20669,9 +20617,8 @@
       <c r="AE39" s="49"/>
       <c r="AF39" s="9"/>
       <c r="AG39" s="9"/>
-      <c r="AH39" s="77"/>
-      <c r="AI39" s="77"/>
-      <c r="AJ39" s="78"/>
+      <c r="AH39" s="9"/>
+      <c r="AI39" s="9"/>
     </row>
     <row r="40" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="73" t="s">
@@ -20767,9 +20714,7 @@
       <c r="AE40" s="49"/>
       <c r="AF40" s="9"/>
       <c r="AG40" s="9"/>
-      <c r="AH40" s="77"/>
-      <c r="AI40" s="78"/>
-      <c r="AJ40" s="78"/>
+      <c r="AH40" s="9"/>
     </row>
     <row r="41" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="73" t="s">
@@ -20865,9 +20810,7 @@
       <c r="AE41" s="49"/>
       <c r="AF41" s="9"/>
       <c r="AG41" s="9"/>
-      <c r="AH41" s="77"/>
-      <c r="AI41" s="78"/>
-      <c r="AJ41" s="78"/>
+      <c r="AH41" s="9"/>
     </row>
     <row r="42" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="73" t="s">
@@ -20990,9 +20933,7 @@
       <c r="AE42" s="51"/>
       <c r="AF42" s="16"/>
       <c r="AG42" s="16"/>
-      <c r="AH42" s="81"/>
-      <c r="AI42" s="78"/>
-      <c r="AJ42" s="78"/>
+      <c r="AH42" s="16"/>
     </row>
     <row r="43" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="7"/>
@@ -21028,9 +20969,7 @@
       <c r="AE43" s="49"/>
       <c r="AF43" s="9"/>
       <c r="AG43" s="9"/>
-      <c r="AH43" s="77"/>
-      <c r="AI43" s="78"/>
-      <c r="AJ43" s="78"/>
+      <c r="AH43" s="9"/>
     </row>
     <row r="44" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="74" t="s">
@@ -21126,9 +21065,8 @@
       <c r="AE44" s="49"/>
       <c r="AF44" s="9"/>
       <c r="AG44" s="9"/>
-      <c r="AH44" s="77"/>
-      <c r="AI44" s="77"/>
-      <c r="AJ44" s="78"/>
+      <c r="AH44" s="9"/>
+      <c r="AI44" s="9"/>
     </row>
     <row r="45" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
@@ -21224,9 +21162,7 @@
       <c r="AE45" s="49"/>
       <c r="AF45" s="9"/>
       <c r="AG45" s="9"/>
-      <c r="AH45" s="77"/>
-      <c r="AI45" s="78"/>
-      <c r="AJ45" s="78"/>
+      <c r="AH45" s="9"/>
     </row>
     <row r="46" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
@@ -21322,9 +21258,8 @@
       <c r="AE46" s="49"/>
       <c r="AF46" s="9"/>
       <c r="AG46" s="9"/>
-      <c r="AH46" s="77"/>
-      <c r="AI46" s="85"/>
-      <c r="AJ46" s="78"/>
+      <c r="AH46" s="9"/>
+      <c r="AI46" s="30"/>
     </row>
     <row r="47" spans="1:36" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="73" t="s">
@@ -21449,9 +21384,8 @@
       <c r="AE47" s="56"/>
       <c r="AF47" s="32"/>
       <c r="AG47" s="32"/>
-      <c r="AH47" s="86"/>
-      <c r="AI47" s="85"/>
-      <c r="AJ47" s="78"/>
+      <c r="AH47" s="32"/>
+      <c r="AJ47"/>
     </row>
     <row r="48" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="73" t="s">
@@ -21547,11 +21481,9 @@
       <c r="AE48" s="49"/>
       <c r="AF48" s="9"/>
       <c r="AG48" s="9"/>
-      <c r="AH48" s="77"/>
-      <c r="AI48" s="78"/>
-      <c r="AJ48" s="78"/>
-    </row>
-    <row r="49" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH48" s="9"/>
+    </row>
+    <row r="49" spans="1:34" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -21585,11 +21517,9 @@
       <c r="AE49" s="49"/>
       <c r="AF49" s="9"/>
       <c r="AG49" s="9"/>
-      <c r="AH49" s="77"/>
-      <c r="AI49" s="78"/>
-      <c r="AJ49" s="78"/>
-    </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AH49" s="9"/>
+    </row>
+    <row r="50" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A50" s="63" t="s">
         <v>38</v>
       </c>
@@ -21625,11 +21555,9 @@
       <c r="AE50" s="49"/>
       <c r="AF50" s="9"/>
       <c r="AG50" s="9"/>
-      <c r="AH50" s="77"/>
-      <c r="AI50" s="78"/>
-      <c r="AJ50" s="78"/>
-    </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AH50" s="9"/>
+    </row>
+    <row r="51" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A51" s="63" t="s">
         <v>39</v>
       </c>
@@ -21671,11 +21599,9 @@
       <c r="AE51" s="49"/>
       <c r="AF51" s="9"/>
       <c r="AG51" s="9"/>
-      <c r="AH51" s="77"/>
-      <c r="AI51" s="78"/>
-      <c r="AJ51" s="78"/>
-    </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AH51" s="9"/>
+    </row>
+    <row r="52" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A52" s="63" t="s">
         <v>40</v>
       </c>
@@ -21713,11 +21639,9 @@
       <c r="AE52" s="49"/>
       <c r="AF52" s="9"/>
       <c r="AG52" s="9"/>
-      <c r="AH52" s="77"/>
-      <c r="AI52" s="78"/>
-      <c r="AJ52" s="78"/>
-    </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AH52" s="9"/>
+    </row>
+    <row r="53" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A53" s="63" t="s">
         <v>41</v>
       </c>
@@ -21753,11 +21677,9 @@
       <c r="AE53" s="49"/>
       <c r="AF53" s="9"/>
       <c r="AG53" s="9"/>
-      <c r="AH53" s="77"/>
-      <c r="AI53" s="78"/>
-      <c r="AJ53" s="78"/>
-    </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AH53" s="9"/>
+    </row>
+    <row r="54" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A54" s="17"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
@@ -21791,11 +21713,9 @@
       <c r="AE54" s="49"/>
       <c r="AF54" s="9"/>
       <c r="AG54" s="9"/>
-      <c r="AH54" s="77"/>
-      <c r="AI54" s="78"/>
-      <c r="AJ54" s="78"/>
-    </row>
-    <row r="55" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+      <c r="AH54" s="9"/>
+    </row>
+    <row r="55" spans="1:34" ht="18" x14ac:dyDescent="0.3">
       <c r="A55" s="75" t="s">
         <v>42</v>
       </c>
@@ -21889,11 +21809,9 @@
       <c r="AE55" s="49"/>
       <c r="AF55" s="9"/>
       <c r="AG55" s="9"/>
-      <c r="AH55" s="77"/>
-      <c r="AI55" s="78"/>
-      <c r="AJ55" s="78"/>
-    </row>
-    <row r="56" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+      <c r="AH55" s="9"/>
+    </row>
+    <row r="56" spans="1:34" ht="18" x14ac:dyDescent="0.3">
       <c r="A56" s="76" t="s">
         <v>43</v>
       </c>
@@ -21987,11 +21905,9 @@
       <c r="AE56" s="49"/>
       <c r="AF56" s="9"/>
       <c r="AG56" s="9"/>
-      <c r="AH56" s="77"/>
-      <c r="AI56" s="78"/>
-      <c r="AJ56" s="78"/>
-    </row>
-    <row r="57" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH56" s="9"/>
+    </row>
+    <row r="57" spans="1:34" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
         <v>44</v>
       </c>
@@ -22027,11 +21943,9 @@
       <c r="AE57" s="49"/>
       <c r="AF57" s="9"/>
       <c r="AG57" s="9"/>
-      <c r="AH57" s="77"/>
-      <c r="AI57" s="78"/>
-      <c r="AJ57" s="78"/>
-    </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AH57" s="9"/>
+    </row>
+    <row r="58" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A58" s="65" t="s">
         <v>45</v>
       </c>
@@ -22125,11 +22039,9 @@
       <c r="AE58" s="49"/>
       <c r="AF58" s="9"/>
       <c r="AG58" s="9"/>
-      <c r="AH58" s="77"/>
-      <c r="AI58" s="78"/>
-      <c r="AJ58" s="78"/>
-    </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AH58" s="9"/>
+    </row>
+    <row r="59" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A59" s="35" t="s">
         <v>46</v>
       </c>
@@ -22223,11 +22135,9 @@
       <c r="AE59" s="49"/>
       <c r="AF59" s="9"/>
       <c r="AG59" s="9"/>
-      <c r="AH59" s="77"/>
-      <c r="AI59" s="78"/>
-      <c r="AJ59" s="78"/>
-    </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AH59" s="9"/>
+    </row>
+    <row r="60" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A60" s="66" t="s">
         <v>47</v>
       </c>
@@ -22321,11 +22231,9 @@
       <c r="AE60" s="49"/>
       <c r="AF60" s="9"/>
       <c r="AG60" s="9"/>
-      <c r="AH60" s="77"/>
-      <c r="AI60" s="78"/>
-      <c r="AJ60" s="78"/>
-    </row>
-    <row r="61" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH60" s="9"/>
+    </row>
+    <row r="61" spans="1:34" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>48</v>
       </c>
@@ -22448,11 +22356,9 @@
       <c r="AE61" s="57"/>
       <c r="AF61" s="62"/>
       <c r="AG61" s="62"/>
-      <c r="AH61" s="87"/>
-      <c r="AI61" s="78"/>
-      <c r="AJ61" s="78"/>
-    </row>
-    <row r="62" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH61" s="37"/>
+    </row>
+    <row r="62" spans="1:34" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="7"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
@@ -22486,11 +22392,9 @@
       <c r="AE62" s="49"/>
       <c r="AF62" s="9"/>
       <c r="AG62" s="9"/>
-      <c r="AH62" s="77"/>
-      <c r="AI62" s="78"/>
-      <c r="AJ62" s="78"/>
-    </row>
-    <row r="63" spans="1:36" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="AH62" s="9"/>
+    </row>
+    <row r="63" spans="1:34" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A63" s="38" t="s">
         <v>49</v>
       </c>
@@ -22580,11 +22484,9 @@
       <c r="AE63" s="49"/>
       <c r="AF63" s="9"/>
       <c r="AG63" s="9"/>
-      <c r="AH63" s="77"/>
-      <c r="AI63" s="78"/>
-      <c r="AJ63" s="78"/>
-    </row>
-    <row r="64" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+      <c r="AH63" s="9"/>
+    </row>
+    <row r="64" spans="1:34" ht="18" x14ac:dyDescent="0.3">
       <c r="A64" s="33" t="s">
         <v>50</v>
       </c>
@@ -22678,11 +22580,9 @@
       <c r="AE64" s="49"/>
       <c r="AF64" s="9"/>
       <c r="AG64" s="9"/>
-      <c r="AH64" s="77"/>
-      <c r="AI64" s="78"/>
-      <c r="AJ64" s="78"/>
-    </row>
-    <row r="65" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+      <c r="AH64" s="9"/>
+    </row>
+    <row r="65" spans="1:35" ht="18" x14ac:dyDescent="0.3">
       <c r="A65" s="64" t="s">
         <v>51</v>
       </c>
@@ -22776,11 +22676,9 @@
       <c r="AE65" s="49"/>
       <c r="AF65" s="9"/>
       <c r="AG65" s="9"/>
-      <c r="AH65" s="77"/>
-      <c r="AI65" s="78"/>
-      <c r="AJ65" s="78"/>
-    </row>
-    <row r="66" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+      <c r="AH65" s="9"/>
+    </row>
+    <row r="66" spans="1:35" ht="18" x14ac:dyDescent="0.3">
       <c r="A66" s="64" t="s">
         <v>69</v>
       </c>
@@ -22901,11 +22799,9 @@
       <c r="AE66" s="51"/>
       <c r="AF66" s="16"/>
       <c r="AG66" s="16"/>
-      <c r="AH66" s="81"/>
-      <c r="AI66" s="78"/>
-      <c r="AJ66" s="78"/>
-    </row>
-    <row r="67" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+      <c r="AH66" s="16"/>
+    </row>
+    <row r="67" spans="1:35" ht="18" x14ac:dyDescent="0.3">
       <c r="A67" s="34"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
@@ -22939,11 +22835,9 @@
       <c r="AE67" s="49"/>
       <c r="AF67" s="9"/>
       <c r="AG67" s="9"/>
-      <c r="AH67" s="77"/>
-      <c r="AI67" s="78"/>
-      <c r="AJ67" s="78"/>
-    </row>
-    <row r="68" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+      <c r="AH67" s="9"/>
+    </row>
+    <row r="68" spans="1:35" ht="18" x14ac:dyDescent="0.3">
       <c r="A68" s="75" t="s">
         <v>52</v>
       </c>
@@ -23037,11 +22931,9 @@
       <c r="AE68" s="49"/>
       <c r="AF68" s="9"/>
       <c r="AG68" s="9"/>
-      <c r="AH68" s="77"/>
-      <c r="AI68" s="78"/>
-      <c r="AJ68" s="78"/>
-    </row>
-    <row r="69" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+      <c r="AH68" s="9"/>
+    </row>
+    <row r="69" spans="1:35" ht="18" x14ac:dyDescent="0.3">
       <c r="A69" s="34"/>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
@@ -23075,11 +22967,9 @@
       <c r="AE69" s="49"/>
       <c r="AF69" s="9"/>
       <c r="AG69" s="9"/>
-      <c r="AH69" s="77"/>
-      <c r="AI69" s="78"/>
-      <c r="AJ69" s="78"/>
-    </row>
-    <row r="70" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+      <c r="AH69" s="9"/>
+    </row>
+    <row r="70" spans="1:35" ht="18" x14ac:dyDescent="0.3">
       <c r="A70" s="33" t="s">
         <v>53</v>
       </c>
@@ -23115,11 +23005,9 @@
       <c r="AE70" s="49"/>
       <c r="AF70" s="9"/>
       <c r="AG70" s="9"/>
-      <c r="AH70" s="77"/>
-      <c r="AI70" s="78"/>
-      <c r="AJ70" s="78"/>
-    </row>
-    <row r="71" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+      <c r="AH70" s="9"/>
+    </row>
+    <row r="71" spans="1:35" ht="18" x14ac:dyDescent="0.3">
       <c r="A71" s="64" t="s">
         <v>54</v>
       </c>
@@ -23213,11 +23101,9 @@
       <c r="AE71" s="58"/>
       <c r="AF71" s="40"/>
       <c r="AG71" s="40"/>
-      <c r="AH71" s="88"/>
-      <c r="AI71" s="78"/>
-      <c r="AJ71" s="78"/>
-    </row>
-    <row r="72" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+      <c r="AH71" s="40"/>
+    </row>
+    <row r="72" spans="1:35" ht="18" x14ac:dyDescent="0.3">
       <c r="A72" s="64" t="s">
         <v>55</v>
       </c>
@@ -23311,11 +23197,9 @@
       <c r="AE72" s="58"/>
       <c r="AF72" s="40"/>
       <c r="AG72" s="40"/>
-      <c r="AH72" s="88"/>
-      <c r="AI72" s="78"/>
-      <c r="AJ72" s="78"/>
-    </row>
-    <row r="73" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+      <c r="AH72" s="40"/>
+    </row>
+    <row r="73" spans="1:35" ht="18" x14ac:dyDescent="0.3">
       <c r="A73" s="34"/>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
@@ -23351,7 +23235,7 @@
       <c r="AG73" s="9"/>
       <c r="AH73" s="9"/>
     </row>
-    <row r="74" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="10" t="s">
         <v>56</v>
       </c>
@@ -23447,7 +23331,7 @@
       <c r="AG74" s="9"/>
       <c r="AH74" s="9"/>
     </row>
-    <row r="75" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="10" t="s">
         <v>57</v>
       </c>
@@ -23543,7 +23427,7 @@
       <c r="AG75" s="9"/>
       <c r="AH75" s="9"/>
     </row>
-    <row r="76" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:35" ht="18" x14ac:dyDescent="0.3">
       <c r="A76" s="33" t="s">
         <v>58</v>
       </c>
@@ -23639,7 +23523,7 @@
       <c r="AG76" s="9"/>
       <c r="AH76" s="9"/>
     </row>
-    <row r="77" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:35" ht="18" x14ac:dyDescent="0.3">
       <c r="A77" s="33" t="s">
         <v>59</v>
       </c>
@@ -23735,7 +23619,7 @@
       <c r="AG77" s="9"/>
       <c r="AH77" s="9"/>
     </row>
-    <row r="78" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:35" ht="18" x14ac:dyDescent="0.3">
       <c r="A78" s="33" t="s">
         <v>68</v>
       </c>
@@ -23818,10 +23702,10 @@
         <v>60</v>
       </c>
     </row>
-    <row r="79" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A79" s="41"/>
     </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A80" s="41"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>